<commit_message>
Updated gantt chart and figures
</commit_message>
<xml_diff>
--- a/Documentation/Reports and Papers/Knee_Torque_Test/Paper Gantt chart.xlsx
+++ b/Documentation/Reports and Papers/Knee_Torque_Test/Paper Gantt chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Bipedal_Robot\Documentation\Reports and Papers\Knee_Torque_Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{06529F2F-7FF4-4BBA-A7E9-658836539885}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9470EB34-2D4A-4976-98F2-4AF21E1A8D91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
     <author>Ben Bolen</author>
   </authors>
   <commentList>
-    <comment ref="B26" authorId="0" shapeId="0" xr:uid="{2E9B2A04-9D58-413F-971B-1FE252920761}">
+    <comment ref="B27" authorId="0" shapeId="0" xr:uid="{2E9B2A04-9D58-413F-971B-1FE252920761}">
       <text>
         <r>
           <rPr>
@@ -65,7 +65,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B27" authorId="0" shapeId="0" xr:uid="{EACBC4D3-8B3B-43AD-B12B-C653980635DF}">
+    <comment ref="B28" authorId="0" shapeId="0" xr:uid="{EACBC4D3-8B3B-43AD-B12B-C653980635DF}">
       <text>
         <r>
           <rPr>
@@ -94,7 +94,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="49">
   <si>
     <t>Insert new rows ABOVE this one</t>
   </si>
@@ -243,6 +243,9 @@
   </si>
   <si>
     <t>Knee Torque paper</t>
+  </si>
+  <si>
+    <t>Update algorithms with new 10,20 mm force equations</t>
   </si>
 </sst>
 </file>
@@ -851,7 +854,7 @@
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="119">
+  <cellXfs count="120">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1178,6 +1181,9 @@
     </xf>
     <xf numFmtId="166" fontId="19" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="5" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -1777,10 +1783,10 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BL35"/>
+  <dimension ref="A1:BL36"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A8" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A18" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1817,7 +1823,7 @@
       <c r="P1" s="24"/>
       <c r="Q1" s="113">
         <f ca="1">TODAY()</f>
-        <v>45260</v>
+        <v>45264</v>
       </c>
       <c r="R1" s="112"/>
       <c r="S1" s="112"/>
@@ -1878,7 +1884,7 @@
       <c r="E4" s="30"/>
       <c r="I4" s="118">
         <f ca="1">I5</f>
-        <v>45257</v>
+        <v>45264</v>
       </c>
       <c r="J4" s="116"/>
       <c r="K4" s="116"/>
@@ -1888,7 +1894,7 @@
       <c r="O4" s="116"/>
       <c r="P4" s="116">
         <f ca="1">P5</f>
-        <v>45264</v>
+        <v>45271</v>
       </c>
       <c r="Q4" s="116"/>
       <c r="R4" s="116"/>
@@ -1898,7 +1904,7 @@
       <c r="V4" s="116"/>
       <c r="W4" s="116">
         <f ca="1">W5</f>
-        <v>45271</v>
+        <v>45278</v>
       </c>
       <c r="X4" s="116"/>
       <c r="Y4" s="116"/>
@@ -1908,7 +1914,7 @@
       <c r="AC4" s="116"/>
       <c r="AD4" s="116">
         <f ca="1">AD5</f>
-        <v>45278</v>
+        <v>45285</v>
       </c>
       <c r="AE4" s="116"/>
       <c r="AF4" s="116"/>
@@ -1918,7 +1924,7 @@
       <c r="AJ4" s="116"/>
       <c r="AK4" s="116">
         <f ca="1">AK5</f>
-        <v>45285</v>
+        <v>45292</v>
       </c>
       <c r="AL4" s="116"/>
       <c r="AM4" s="116"/>
@@ -1928,7 +1934,7 @@
       <c r="AQ4" s="116"/>
       <c r="AR4" s="116">
         <f ca="1">AR5</f>
-        <v>45292</v>
+        <v>45299</v>
       </c>
       <c r="AS4" s="116"/>
       <c r="AT4" s="116"/>
@@ -1938,7 +1944,7 @@
       <c r="AX4" s="116"/>
       <c r="AY4" s="116">
         <f ca="1">AY5</f>
-        <v>45299</v>
+        <v>45306</v>
       </c>
       <c r="AZ4" s="116"/>
       <c r="BA4" s="116"/>
@@ -1948,7 +1954,7 @@
       <c r="BE4" s="116"/>
       <c r="BF4" s="116">
         <f ca="1">BF5</f>
-        <v>45306</v>
+        <v>45313</v>
       </c>
       <c r="BG4" s="116"/>
       <c r="BH4" s="116"/>
@@ -1976,227 +1982,227 @@
       </c>
       <c r="I5" s="31">
         <f ca="1">Project_Start-WEEKDAY(Project_Start,1)+2+7*(Display_Week-1)</f>
-        <v>45257</v>
+        <v>45264</v>
       </c>
       <c r="J5" s="31">
         <f ca="1">I5+1</f>
-        <v>45258</v>
+        <v>45265</v>
       </c>
       <c r="K5" s="31">
         <f t="shared" ref="K5:AX5" ca="1" si="0">J5+1</f>
-        <v>45259</v>
+        <v>45266</v>
       </c>
       <c r="L5" s="31">
         <f t="shared" ca="1" si="0"/>
-        <v>45260</v>
+        <v>45267</v>
       </c>
       <c r="M5" s="31">
         <f t="shared" ca="1" si="0"/>
-        <v>45261</v>
+        <v>45268</v>
       </c>
       <c r="N5" s="31">
         <f t="shared" ca="1" si="0"/>
-        <v>45262</v>
+        <v>45269</v>
       </c>
       <c r="O5" s="32">
         <f t="shared" ca="1" si="0"/>
-        <v>45263</v>
+        <v>45270</v>
       </c>
       <c r="P5" s="33">
         <f ca="1">O5+1</f>
-        <v>45264</v>
+        <v>45271</v>
       </c>
       <c r="Q5" s="31">
         <f ca="1">P5+1</f>
-        <v>45265</v>
+        <v>45272</v>
       </c>
       <c r="R5" s="31">
         <f t="shared" ca="1" si="0"/>
-        <v>45266</v>
+        <v>45273</v>
       </c>
       <c r="S5" s="31">
         <f t="shared" ca="1" si="0"/>
-        <v>45267</v>
+        <v>45274</v>
       </c>
       <c r="T5" s="31">
         <f t="shared" ca="1" si="0"/>
-        <v>45268</v>
+        <v>45275</v>
       </c>
       <c r="U5" s="31">
         <f t="shared" ca="1" si="0"/>
-        <v>45269</v>
+        <v>45276</v>
       </c>
       <c r="V5" s="32">
         <f t="shared" ca="1" si="0"/>
-        <v>45270</v>
+        <v>45277</v>
       </c>
       <c r="W5" s="33">
         <f ca="1">V5+1</f>
-        <v>45271</v>
+        <v>45278</v>
       </c>
       <c r="X5" s="31">
         <f ca="1">W5+1</f>
-        <v>45272</v>
+        <v>45279</v>
       </c>
       <c r="Y5" s="31">
         <f t="shared" ca="1" si="0"/>
-        <v>45273</v>
+        <v>45280</v>
       </c>
       <c r="Z5" s="31">
         <f t="shared" ca="1" si="0"/>
-        <v>45274</v>
+        <v>45281</v>
       </c>
       <c r="AA5" s="31">
         <f t="shared" ca="1" si="0"/>
-        <v>45275</v>
+        <v>45282</v>
       </c>
       <c r="AB5" s="31">
         <f t="shared" ca="1" si="0"/>
-        <v>45276</v>
+        <v>45283</v>
       </c>
       <c r="AC5" s="32">
         <f t="shared" ca="1" si="0"/>
-        <v>45277</v>
+        <v>45284</v>
       </c>
       <c r="AD5" s="33">
         <f ca="1">AC5+1</f>
-        <v>45278</v>
+        <v>45285</v>
       </c>
       <c r="AE5" s="31">
         <f ca="1">AD5+1</f>
-        <v>45279</v>
+        <v>45286</v>
       </c>
       <c r="AF5" s="31">
         <f t="shared" ca="1" si="0"/>
-        <v>45280</v>
+        <v>45287</v>
       </c>
       <c r="AG5" s="31">
         <f t="shared" ca="1" si="0"/>
-        <v>45281</v>
+        <v>45288</v>
       </c>
       <c r="AH5" s="31">
         <f t="shared" ca="1" si="0"/>
-        <v>45282</v>
+        <v>45289</v>
       </c>
       <c r="AI5" s="31">
         <f t="shared" ca="1" si="0"/>
-        <v>45283</v>
+        <v>45290</v>
       </c>
       <c r="AJ5" s="32">
         <f t="shared" ca="1" si="0"/>
-        <v>45284</v>
+        <v>45291</v>
       </c>
       <c r="AK5" s="33">
         <f ca="1">AJ5+1</f>
-        <v>45285</v>
+        <v>45292</v>
       </c>
       <c r="AL5" s="31">
         <f ca="1">AK5+1</f>
-        <v>45286</v>
+        <v>45293</v>
       </c>
       <c r="AM5" s="31">
         <f t="shared" ca="1" si="0"/>
-        <v>45287</v>
+        <v>45294</v>
       </c>
       <c r="AN5" s="31">
         <f t="shared" ca="1" si="0"/>
-        <v>45288</v>
+        <v>45295</v>
       </c>
       <c r="AO5" s="31">
         <f t="shared" ca="1" si="0"/>
-        <v>45289</v>
+        <v>45296</v>
       </c>
       <c r="AP5" s="31">
         <f t="shared" ca="1" si="0"/>
-        <v>45290</v>
+        <v>45297</v>
       </c>
       <c r="AQ5" s="32">
         <f t="shared" ca="1" si="0"/>
-        <v>45291</v>
+        <v>45298</v>
       </c>
       <c r="AR5" s="33">
         <f ca="1">AQ5+1</f>
-        <v>45292</v>
+        <v>45299</v>
       </c>
       <c r="AS5" s="31">
         <f ca="1">AR5+1</f>
-        <v>45293</v>
+        <v>45300</v>
       </c>
       <c r="AT5" s="31">
         <f t="shared" ca="1" si="0"/>
-        <v>45294</v>
+        <v>45301</v>
       </c>
       <c r="AU5" s="31">
         <f t="shared" ca="1" si="0"/>
-        <v>45295</v>
+        <v>45302</v>
       </c>
       <c r="AV5" s="31">
         <f t="shared" ca="1" si="0"/>
-        <v>45296</v>
+        <v>45303</v>
       </c>
       <c r="AW5" s="31">
         <f t="shared" ca="1" si="0"/>
-        <v>45297</v>
+        <v>45304</v>
       </c>
       <c r="AX5" s="32">
         <f t="shared" ca="1" si="0"/>
-        <v>45298</v>
+        <v>45305</v>
       </c>
       <c r="AY5" s="33">
         <f ca="1">AX5+1</f>
-        <v>45299</v>
+        <v>45306</v>
       </c>
       <c r="AZ5" s="31">
         <f ca="1">AY5+1</f>
-        <v>45300</v>
+        <v>45307</v>
       </c>
       <c r="BA5" s="31">
         <f t="shared" ref="BA5:BE5" ca="1" si="1">AZ5+1</f>
-        <v>45301</v>
+        <v>45308</v>
       </c>
       <c r="BB5" s="31">
         <f t="shared" ca="1" si="1"/>
-        <v>45302</v>
+        <v>45309</v>
       </c>
       <c r="BC5" s="31">
         <f t="shared" ca="1" si="1"/>
-        <v>45303</v>
+        <v>45310</v>
       </c>
       <c r="BD5" s="31">
         <f t="shared" ca="1" si="1"/>
-        <v>45304</v>
+        <v>45311</v>
       </c>
       <c r="BE5" s="32">
         <f t="shared" ca="1" si="1"/>
-        <v>45305</v>
+        <v>45312</v>
       </c>
       <c r="BF5" s="33">
         <f ca="1">BE5+1</f>
-        <v>45306</v>
+        <v>45313</v>
       </c>
       <c r="BG5" s="31">
         <f ca="1">BF5+1</f>
-        <v>45307</v>
+        <v>45314</v>
       </c>
       <c r="BH5" s="31">
         <f t="shared" ref="BH5:BL5" ca="1" si="2">BG5+1</f>
-        <v>45308</v>
+        <v>45315</v>
       </c>
       <c r="BI5" s="31">
         <f t="shared" ca="1" si="2"/>
-        <v>45309</v>
+        <v>45316</v>
       </c>
       <c r="BJ5" s="31">
         <f t="shared" ca="1" si="2"/>
-        <v>45310</v>
+        <v>45317</v>
       </c>
       <c r="BK5" s="31">
         <f t="shared" ca="1" si="2"/>
-        <v>45311</v>
+        <v>45318</v>
       </c>
       <c r="BL5" s="31">
         <f t="shared" ca="1" si="2"/>
-        <v>45312</v>
+        <v>45319</v>
       </c>
     </row>
     <row r="6" spans="1:64" s="26" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -2512,7 +2518,7 @@
       <c r="F8" s="44"/>
       <c r="G8" s="17"/>
       <c r="H8" s="5" t="str">
-        <f t="shared" ref="H8:H32" si="5">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
+        <f t="shared" ref="H8:H33" si="5">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v/>
       </c>
       <c r="I8" s="45"/>
@@ -2585,7 +2591,7 @@
       </c>
       <c r="E9" s="50">
         <f ca="1">Project_Start</f>
-        <v>45260</v>
+        <v>45264</v>
       </c>
       <c r="F9" s="50">
         <v>45278</v>
@@ -2593,7 +2599,7 @@
       <c r="G9" s="17"/>
       <c r="H9" s="5">
         <f t="shared" ca="1" si="5"/>
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="I9" s="51"/>
       <c r="J9" s="51"/>
@@ -2828,8 +2834,8 @@
     </row>
     <row r="13" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="14"/>
-      <c r="B13" s="61" t="s">
-        <v>33</v>
+      <c r="B13" s="119" t="s">
+        <v>48</v>
       </c>
       <c r="C13" s="62" t="s">
         <v>26</v>
@@ -2841,12 +2847,12 @@
         <v>45262</v>
       </c>
       <c r="F13" s="64">
-        <v>45263</v>
+        <v>45264</v>
       </c>
       <c r="G13" s="17"/>
       <c r="H13" s="5">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I13" s="51"/>
       <c r="J13" s="51"/>
@@ -2906,21 +2912,23 @@
       <c r="BL13" s="51"/>
     </row>
     <row r="14" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="13"/>
+      <c r="A14" s="14"/>
       <c r="B14" s="61" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C14" s="62" t="s">
         <v>26</v>
       </c>
       <c r="D14" s="63">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="E14" s="64">
-        <v>45262</v>
+        <f>F13</f>
+        <v>45264</v>
       </c>
       <c r="F14" s="64">
-        <v>45263</v>
+        <f>E14+1</f>
+        <v>45265</v>
       </c>
       <c r="G14" s="17"/>
       <c r="H14" s="5">
@@ -2939,8 +2947,8 @@
       <c r="R14" s="51"/>
       <c r="S14" s="51"/>
       <c r="T14" s="51"/>
-      <c r="U14" s="55"/>
-      <c r="V14" s="55"/>
+      <c r="U14" s="51"/>
+      <c r="V14" s="51"/>
       <c r="W14" s="51"/>
       <c r="X14" s="51"/>
       <c r="Y14" s="51"/>
@@ -2987,22 +2995,25 @@
     <row r="15" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="13"/>
       <c r="B15" s="61" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C15" s="62" t="s">
         <v>26</v>
       </c>
-      <c r="D15" s="63"/>
+      <c r="D15" s="63">
+        <v>0</v>
+      </c>
       <c r="E15" s="64">
-        <v>45263</v>
+        <v>45262</v>
       </c>
       <c r="F15" s="64">
-        <v>45264</v>
+        <f>F14+1</f>
+        <v>45266</v>
       </c>
       <c r="G15" s="17"/>
       <c r="H15" s="5">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I15" s="51"/>
       <c r="J15" s="51"/>
@@ -3016,8 +3027,8 @@
       <c r="R15" s="51"/>
       <c r="S15" s="51"/>
       <c r="T15" s="51"/>
-      <c r="U15" s="51"/>
-      <c r="V15" s="51"/>
+      <c r="U15" s="55"/>
+      <c r="V15" s="55"/>
       <c r="W15" s="51"/>
       <c r="X15" s="51"/>
       <c r="Y15" s="51"/>
@@ -3064,22 +3075,24 @@
     <row r="16" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="13"/>
       <c r="B16" s="61" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C16" s="62" t="s">
         <v>26</v>
       </c>
       <c r="D16" s="63"/>
       <c r="E16" s="64">
-        <v>45264</v>
+        <f>F15</f>
+        <v>45266</v>
       </c>
       <c r="F16" s="64">
-        <v>45266</v>
+        <f>E16+1</f>
+        <v>45267</v>
       </c>
       <c r="G16" s="17"/>
       <c r="H16" s="5">
         <f t="shared" si="5"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I16" s="51"/>
       <c r="J16" s="51"/>
@@ -3097,7 +3110,7 @@
       <c r="V16" s="51"/>
       <c r="W16" s="51"/>
       <c r="X16" s="51"/>
-      <c r="Y16" s="55"/>
+      <c r="Y16" s="51"/>
       <c r="Z16" s="51"/>
       <c r="AA16" s="51"/>
       <c r="AB16" s="51"/>
@@ -3141,24 +3154,24 @@
     <row r="17" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="13"/>
       <c r="B17" s="61" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="C17" s="62" t="s">
         <v>26</v>
       </c>
       <c r="D17" s="63"/>
       <c r="E17" s="64">
-        <f>E13</f>
-        <v>45262</v>
+        <f>F16</f>
+        <v>45267</v>
       </c>
       <c r="F17" s="64">
-        <f>F16</f>
-        <v>45266</v>
+        <f>E17+1</f>
+        <v>45268</v>
       </c>
       <c r="G17" s="17"/>
       <c r="H17" s="5">
         <f t="shared" si="5"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I17" s="51"/>
       <c r="J17" s="51"/>
@@ -3176,7 +3189,7 @@
       <c r="V17" s="51"/>
       <c r="W17" s="51"/>
       <c r="X17" s="51"/>
-      <c r="Y17" s="51"/>
+      <c r="Y17" s="55"/>
       <c r="Z17" s="51"/>
       <c r="AA17" s="51"/>
       <c r="AB17" s="51"/>
@@ -3219,160 +3232,158 @@
     </row>
     <row r="18" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="13"/>
-      <c r="B18" s="65" t="s">
+      <c r="B18" s="61" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" s="62" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" s="63"/>
+      <c r="E18" s="64">
+        <f>E13</f>
+        <v>45262</v>
+      </c>
+      <c r="F18" s="64">
+        <f>F17</f>
+        <v>45268</v>
+      </c>
+      <c r="G18" s="17"/>
+      <c r="H18" s="5">
+        <f t="shared" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="I18" s="51"/>
+      <c r="J18" s="51"/>
+      <c r="K18" s="51"/>
+      <c r="L18" s="51"/>
+      <c r="M18" s="51"/>
+      <c r="N18" s="51"/>
+      <c r="O18" s="51"/>
+      <c r="P18" s="51"/>
+      <c r="Q18" s="51"/>
+      <c r="R18" s="51"/>
+      <c r="S18" s="51"/>
+      <c r="T18" s="51"/>
+      <c r="U18" s="51"/>
+      <c r="V18" s="51"/>
+      <c r="W18" s="51"/>
+      <c r="X18" s="51"/>
+      <c r="Y18" s="51"/>
+      <c r="Z18" s="51"/>
+      <c r="AA18" s="51"/>
+      <c r="AB18" s="51"/>
+      <c r="AC18" s="51"/>
+      <c r="AD18" s="51"/>
+      <c r="AE18" s="51"/>
+      <c r="AF18" s="51"/>
+      <c r="AG18" s="51"/>
+      <c r="AH18" s="51"/>
+      <c r="AI18" s="51"/>
+      <c r="AJ18" s="51"/>
+      <c r="AK18" s="51"/>
+      <c r="AL18" s="51"/>
+      <c r="AM18" s="51"/>
+      <c r="AN18" s="51"/>
+      <c r="AO18" s="51"/>
+      <c r="AP18" s="51"/>
+      <c r="AQ18" s="51"/>
+      <c r="AR18" s="51"/>
+      <c r="AS18" s="51"/>
+      <c r="AT18" s="51"/>
+      <c r="AU18" s="51"/>
+      <c r="AV18" s="51"/>
+      <c r="AW18" s="51"/>
+      <c r="AX18" s="51"/>
+      <c r="AY18" s="51"/>
+      <c r="AZ18" s="51"/>
+      <c r="BA18" s="51"/>
+      <c r="BB18" s="51"/>
+      <c r="BC18" s="51"/>
+      <c r="BD18" s="51"/>
+      <c r="BE18" s="51"/>
+      <c r="BF18" s="51"/>
+      <c r="BG18" s="51"/>
+      <c r="BH18" s="51"/>
+      <c r="BI18" s="51"/>
+      <c r="BJ18" s="51"/>
+      <c r="BK18" s="51"/>
+      <c r="BL18" s="51"/>
+    </row>
+    <row r="19" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="13"/>
+      <c r="B19" s="65" t="s">
         <v>31</v>
       </c>
-      <c r="C18" s="66"/>
-      <c r="D18" s="67"/>
-      <c r="E18" s="68"/>
-      <c r="F18" s="69"/>
-      <c r="G18" s="17"/>
-      <c r="H18" s="5" t="str">
+      <c r="C19" s="66"/>
+      <c r="D19" s="67"/>
+      <c r="E19" s="68"/>
+      <c r="F19" s="69"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="5" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="I18" s="70"/>
-      <c r="J18" s="70"/>
-      <c r="K18" s="70"/>
-      <c r="L18" s="70"/>
-      <c r="M18" s="70"/>
-      <c r="N18" s="70"/>
-      <c r="O18" s="70"/>
-      <c r="P18" s="70"/>
-      <c r="Q18" s="70"/>
-      <c r="R18" s="70"/>
-      <c r="S18" s="70"/>
-      <c r="T18" s="70"/>
-      <c r="U18" s="70"/>
-      <c r="V18" s="70"/>
-      <c r="W18" s="70"/>
-      <c r="X18" s="70"/>
-      <c r="Y18" s="70"/>
-      <c r="Z18" s="70"/>
-      <c r="AA18" s="70"/>
-      <c r="AB18" s="70"/>
-      <c r="AC18" s="70"/>
-      <c r="AD18" s="70"/>
-      <c r="AE18" s="70"/>
-      <c r="AF18" s="70"/>
-      <c r="AG18" s="70"/>
-      <c r="AH18" s="70"/>
-      <c r="AI18" s="70"/>
-      <c r="AJ18" s="70"/>
-      <c r="AK18" s="70"/>
-      <c r="AL18" s="70"/>
-      <c r="AM18" s="70"/>
-      <c r="AN18" s="70"/>
-      <c r="AO18" s="70"/>
-      <c r="AP18" s="70"/>
-      <c r="AQ18" s="70"/>
-      <c r="AR18" s="70"/>
-      <c r="AS18" s="70"/>
-      <c r="AT18" s="70"/>
-      <c r="AU18" s="70"/>
-      <c r="AV18" s="70"/>
-      <c r="AW18" s="70"/>
-      <c r="AX18" s="70"/>
-      <c r="AY18" s="70"/>
-      <c r="AZ18" s="70"/>
-      <c r="BA18" s="70"/>
-      <c r="BB18" s="70"/>
-      <c r="BC18" s="70"/>
-      <c r="BD18" s="70"/>
-      <c r="BE18" s="70"/>
-      <c r="BF18" s="70"/>
-      <c r="BG18" s="70"/>
-      <c r="BH18" s="70"/>
-      <c r="BI18" s="70"/>
-      <c r="BJ18" s="70"/>
-      <c r="BK18" s="70"/>
-      <c r="BL18" s="70"/>
-    </row>
-    <row r="19" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="13"/>
-      <c r="B19" s="71" t="s">
-        <v>44</v>
-      </c>
-      <c r="C19" s="72" t="s">
-        <v>26</v>
-      </c>
-      <c r="D19" s="73">
-        <v>0.02</v>
-      </c>
-      <c r="E19" s="74">
-        <f ca="1">TODAY()</f>
-        <v>45260</v>
-      </c>
-      <c r="F19" s="74">
-        <f ca="1">E19+5</f>
-        <v>45265</v>
-      </c>
-      <c r="G19" s="17"/>
-      <c r="H19" s="5">
-        <f t="shared" ca="1" si="5"/>
-        <v>6</v>
-      </c>
-      <c r="I19" s="51"/>
-      <c r="J19" s="51"/>
-      <c r="K19" s="51"/>
-      <c r="L19" s="51"/>
-      <c r="M19" s="51"/>
-      <c r="N19" s="51"/>
-      <c r="O19" s="51"/>
-      <c r="P19" s="51"/>
-      <c r="Q19" s="51"/>
-      <c r="R19" s="51"/>
-      <c r="S19" s="51"/>
-      <c r="T19" s="51"/>
-      <c r="U19" s="51"/>
-      <c r="V19" s="51"/>
-      <c r="W19" s="51"/>
-      <c r="X19" s="51"/>
-      <c r="Y19" s="51"/>
-      <c r="Z19" s="51"/>
-      <c r="AA19" s="51"/>
-      <c r="AB19" s="51"/>
-      <c r="AC19" s="51"/>
-      <c r="AD19" s="51"/>
-      <c r="AE19" s="51"/>
-      <c r="AF19" s="51"/>
-      <c r="AG19" s="51"/>
-      <c r="AH19" s="51"/>
-      <c r="AI19" s="51"/>
-      <c r="AJ19" s="51"/>
-      <c r="AK19" s="51"/>
-      <c r="AL19" s="51"/>
-      <c r="AM19" s="51"/>
-      <c r="AN19" s="51"/>
-      <c r="AO19" s="51"/>
-      <c r="AP19" s="51"/>
-      <c r="AQ19" s="51"/>
-      <c r="AR19" s="51"/>
-      <c r="AS19" s="51"/>
-      <c r="AT19" s="51"/>
-      <c r="AU19" s="51"/>
-      <c r="AV19" s="51"/>
-      <c r="AW19" s="51"/>
-      <c r="AX19" s="51"/>
-      <c r="AY19" s="51"/>
-      <c r="AZ19" s="51"/>
-      <c r="BA19" s="51"/>
-      <c r="BB19" s="51"/>
-      <c r="BC19" s="51"/>
-      <c r="BD19" s="51"/>
-      <c r="BE19" s="51"/>
-      <c r="BF19" s="51"/>
-      <c r="BG19" s="51"/>
-      <c r="BH19" s="51"/>
-      <c r="BI19" s="51"/>
-      <c r="BJ19" s="51"/>
-      <c r="BK19" s="51"/>
-      <c r="BL19" s="51"/>
+      <c r="I19" s="70"/>
+      <c r="J19" s="70"/>
+      <c r="K19" s="70"/>
+      <c r="L19" s="70"/>
+      <c r="M19" s="70"/>
+      <c r="N19" s="70"/>
+      <c r="O19" s="70"/>
+      <c r="P19" s="70"/>
+      <c r="Q19" s="70"/>
+      <c r="R19" s="70"/>
+      <c r="S19" s="70"/>
+      <c r="T19" s="70"/>
+      <c r="U19" s="70"/>
+      <c r="V19" s="70"/>
+      <c r="W19" s="70"/>
+      <c r="X19" s="70"/>
+      <c r="Y19" s="70"/>
+      <c r="Z19" s="70"/>
+      <c r="AA19" s="70"/>
+      <c r="AB19" s="70"/>
+      <c r="AC19" s="70"/>
+      <c r="AD19" s="70"/>
+      <c r="AE19" s="70"/>
+      <c r="AF19" s="70"/>
+      <c r="AG19" s="70"/>
+      <c r="AH19" s="70"/>
+      <c r="AI19" s="70"/>
+      <c r="AJ19" s="70"/>
+      <c r="AK19" s="70"/>
+      <c r="AL19" s="70"/>
+      <c r="AM19" s="70"/>
+      <c r="AN19" s="70"/>
+      <c r="AO19" s="70"/>
+      <c r="AP19" s="70"/>
+      <c r="AQ19" s="70"/>
+      <c r="AR19" s="70"/>
+      <c r="AS19" s="70"/>
+      <c r="AT19" s="70"/>
+      <c r="AU19" s="70"/>
+      <c r="AV19" s="70"/>
+      <c r="AW19" s="70"/>
+      <c r="AX19" s="70"/>
+      <c r="AY19" s="70"/>
+      <c r="AZ19" s="70"/>
+      <c r="BA19" s="70"/>
+      <c r="BB19" s="70"/>
+      <c r="BC19" s="70"/>
+      <c r="BD19" s="70"/>
+      <c r="BE19" s="70"/>
+      <c r="BF19" s="70"/>
+      <c r="BG19" s="70"/>
+      <c r="BH19" s="70"/>
+      <c r="BI19" s="70"/>
+      <c r="BJ19" s="70"/>
+      <c r="BK19" s="70"/>
+      <c r="BL19" s="70"/>
     </row>
     <row r="20" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="13"/>
       <c r="B20" s="71" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="C20" s="72" t="s">
         <v>26</v>
@@ -3382,11 +3393,11 @@
       </c>
       <c r="E20" s="74">
         <f ca="1">TODAY()</f>
-        <v>45260</v>
+        <v>45264</v>
       </c>
       <c r="F20" s="74">
         <f ca="1">E20+5</f>
-        <v>45265</v>
+        <v>45269</v>
       </c>
       <c r="G20" s="17"/>
       <c r="H20" s="5">
@@ -3453,7 +3464,7 @@
     <row r="21" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="13"/>
       <c r="B21" s="71" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C21" s="72" t="s">
         <v>26</v>
@@ -3462,17 +3473,17 @@
         <v>0.02</v>
       </c>
       <c r="E21" s="74">
-        <f ca="1">F20+1</f>
-        <v>45266</v>
+        <f ca="1">TODAY()</f>
+        <v>45264</v>
       </c>
       <c r="F21" s="74">
-        <f ca="1">E21+2</f>
-        <v>45268</v>
+        <f ca="1">E21+5</f>
+        <v>45269</v>
       </c>
       <c r="G21" s="17"/>
       <c r="H21" s="5">
         <f t="shared" ca="1" si="5"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I21" s="51"/>
       <c r="J21" s="51"/>
@@ -3534,21 +3545,21 @@
     <row r="22" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="13"/>
       <c r="B22" s="71" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C22" s="72" t="s">
         <v>26</v>
       </c>
       <c r="D22" s="73">
-        <v>0.5</v>
+        <v>0.02</v>
       </c>
       <c r="E22" s="74">
-        <f ca="1">F29</f>
-        <v>45269</v>
+        <f ca="1">F21+1</f>
+        <v>45270</v>
       </c>
       <c r="F22" s="74">
         <f ca="1">E22+2</f>
-        <v>45271</v>
+        <v>45272</v>
       </c>
       <c r="G22" s="17"/>
       <c r="H22" s="5">
@@ -3615,21 +3626,21 @@
     <row r="23" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="13"/>
       <c r="B23" s="71" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C23" s="72" t="s">
         <v>26</v>
       </c>
       <c r="D23" s="73">
-        <v>0.05</v>
+        <v>0.5</v>
       </c>
       <c r="E23" s="74">
-        <f ca="1">F22</f>
-        <v>45271</v>
+        <f ca="1">F30</f>
+        <v>45273</v>
       </c>
       <c r="F23" s="74">
         <f ca="1">E23+2</f>
-        <v>45273</v>
+        <v>45275</v>
       </c>
       <c r="G23" s="17"/>
       <c r="H23" s="5">
@@ -3696,26 +3707,26 @@
     <row r="24" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="13"/>
       <c r="B24" s="71" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C24" s="72" t="s">
         <v>26</v>
       </c>
       <c r="D24" s="73">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="E24" s="74">
-        <f ca="1">E20</f>
-        <v>45260</v>
+        <f ca="1">F23</f>
+        <v>45275</v>
       </c>
       <c r="F24" s="74">
-        <f ca="1">F23</f>
-        <v>45273</v>
+        <f ca="1">E24+2</f>
+        <v>45277</v>
       </c>
       <c r="G24" s="17"/>
       <c r="H24" s="5">
         <f t="shared" ca="1" si="5"/>
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="I24" s="51"/>
       <c r="J24" s="51"/>
@@ -3776,160 +3787,160 @@
     </row>
     <row r="25" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="13"/>
-      <c r="B25" s="75" t="s">
+      <c r="B25" s="71" t="s">
+        <v>43</v>
+      </c>
+      <c r="C25" s="72" t="s">
+        <v>26</v>
+      </c>
+      <c r="D25" s="73">
+        <v>0</v>
+      </c>
+      <c r="E25" s="74">
+        <f ca="1">E21</f>
+        <v>45264</v>
+      </c>
+      <c r="F25" s="74">
+        <f ca="1">F24</f>
+        <v>45277</v>
+      </c>
+      <c r="G25" s="17"/>
+      <c r="H25" s="5">
+        <f t="shared" ca="1" si="5"/>
+        <v>14</v>
+      </c>
+      <c r="I25" s="51"/>
+      <c r="J25" s="51"/>
+      <c r="K25" s="51"/>
+      <c r="L25" s="51"/>
+      <c r="M25" s="51"/>
+      <c r="N25" s="51"/>
+      <c r="O25" s="51"/>
+      <c r="P25" s="51"/>
+      <c r="Q25" s="51"/>
+      <c r="R25" s="51"/>
+      <c r="S25" s="51"/>
+      <c r="T25" s="51"/>
+      <c r="U25" s="51"/>
+      <c r="V25" s="51"/>
+      <c r="W25" s="51"/>
+      <c r="X25" s="51"/>
+      <c r="Y25" s="51"/>
+      <c r="Z25" s="51"/>
+      <c r="AA25" s="51"/>
+      <c r="AB25" s="51"/>
+      <c r="AC25" s="51"/>
+      <c r="AD25" s="51"/>
+      <c r="AE25" s="51"/>
+      <c r="AF25" s="51"/>
+      <c r="AG25" s="51"/>
+      <c r="AH25" s="51"/>
+      <c r="AI25" s="51"/>
+      <c r="AJ25" s="51"/>
+      <c r="AK25" s="51"/>
+      <c r="AL25" s="51"/>
+      <c r="AM25" s="51"/>
+      <c r="AN25" s="51"/>
+      <c r="AO25" s="51"/>
+      <c r="AP25" s="51"/>
+      <c r="AQ25" s="51"/>
+      <c r="AR25" s="51"/>
+      <c r="AS25" s="51"/>
+      <c r="AT25" s="51"/>
+      <c r="AU25" s="51"/>
+      <c r="AV25" s="51"/>
+      <c r="AW25" s="51"/>
+      <c r="AX25" s="51"/>
+      <c r="AY25" s="51"/>
+      <c r="AZ25" s="51"/>
+      <c r="BA25" s="51"/>
+      <c r="BB25" s="51"/>
+      <c r="BC25" s="51"/>
+      <c r="BD25" s="51"/>
+      <c r="BE25" s="51"/>
+      <c r="BF25" s="51"/>
+      <c r="BG25" s="51"/>
+      <c r="BH25" s="51"/>
+      <c r="BI25" s="51"/>
+      <c r="BJ25" s="51"/>
+      <c r="BK25" s="51"/>
+      <c r="BL25" s="51"/>
+    </row>
+    <row r="26" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="13"/>
+      <c r="B26" s="75" t="s">
         <v>32</v>
       </c>
-      <c r="C25" s="76"/>
-      <c r="D25" s="77"/>
-      <c r="E25" s="78"/>
-      <c r="F25" s="79"/>
-      <c r="G25" s="17"/>
-      <c r="H25" s="5" t="str">
+      <c r="C26" s="76"/>
+      <c r="D26" s="77"/>
+      <c r="E26" s="78"/>
+      <c r="F26" s="79"/>
+      <c r="G26" s="17"/>
+      <c r="H26" s="5" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="I25" s="80"/>
-      <c r="J25" s="80"/>
-      <c r="K25" s="80"/>
-      <c r="L25" s="80"/>
-      <c r="M25" s="80"/>
-      <c r="N25" s="80"/>
-      <c r="O25" s="80"/>
-      <c r="P25" s="80"/>
-      <c r="Q25" s="80"/>
-      <c r="R25" s="80"/>
-      <c r="S25" s="80"/>
-      <c r="T25" s="80"/>
-      <c r="U25" s="80"/>
-      <c r="V25" s="80"/>
-      <c r="W25" s="80"/>
-      <c r="X25" s="80"/>
-      <c r="Y25" s="80"/>
-      <c r="Z25" s="80"/>
-      <c r="AA25" s="80"/>
-      <c r="AB25" s="80"/>
-      <c r="AC25" s="80"/>
-      <c r="AD25" s="80"/>
-      <c r="AE25" s="80"/>
-      <c r="AF25" s="80"/>
-      <c r="AG25" s="80"/>
-      <c r="AH25" s="80"/>
-      <c r="AI25" s="80"/>
-      <c r="AJ25" s="80"/>
-      <c r="AK25" s="80"/>
-      <c r="AL25" s="80"/>
-      <c r="AM25" s="80"/>
-      <c r="AN25" s="80"/>
-      <c r="AO25" s="80"/>
-      <c r="AP25" s="80"/>
-      <c r="AQ25" s="80"/>
-      <c r="AR25" s="80"/>
-      <c r="AS25" s="80"/>
-      <c r="AT25" s="80"/>
-      <c r="AU25" s="80"/>
-      <c r="AV25" s="80"/>
-      <c r="AW25" s="80"/>
-      <c r="AX25" s="80"/>
-      <c r="AY25" s="80"/>
-      <c r="AZ25" s="80"/>
-      <c r="BA25" s="80"/>
-      <c r="BB25" s="80"/>
-      <c r="BC25" s="80"/>
-      <c r="BD25" s="80"/>
-      <c r="BE25" s="80"/>
-      <c r="BF25" s="80"/>
-      <c r="BG25" s="80"/>
-      <c r="BH25" s="80"/>
-      <c r="BI25" s="80"/>
-      <c r="BJ25" s="80"/>
-      <c r="BK25" s="80"/>
-      <c r="BL25" s="80"/>
-    </row>
-    <row r="26" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="13"/>
-      <c r="B26" s="81" t="s">
-        <v>41</v>
-      </c>
-      <c r="C26" s="82" t="s">
-        <v>26</v>
-      </c>
-      <c r="D26" s="83">
-        <v>0.05</v>
-      </c>
-      <c r="E26" s="84">
-        <f ca="1">E20+2</f>
-        <v>45262</v>
-      </c>
-      <c r="F26" s="84">
-        <f ca="1">E26+3</f>
-        <v>45265</v>
-      </c>
-      <c r="G26" s="17"/>
-      <c r="H26" s="5">
-        <f t="shared" ca="1" si="5"/>
-        <v>4</v>
-      </c>
-      <c r="I26" s="51"/>
-      <c r="J26" s="51"/>
-      <c r="K26" s="51"/>
-      <c r="L26" s="51"/>
-      <c r="M26" s="51"/>
-      <c r="N26" s="51"/>
-      <c r="O26" s="51"/>
-      <c r="P26" s="51"/>
-      <c r="Q26" s="51"/>
-      <c r="R26" s="51"/>
-      <c r="S26" s="51"/>
-      <c r="T26" s="51"/>
-      <c r="U26" s="51"/>
-      <c r="V26" s="51"/>
-      <c r="W26" s="51"/>
-      <c r="X26" s="51"/>
-      <c r="Y26" s="51"/>
-      <c r="Z26" s="51"/>
-      <c r="AA26" s="51"/>
-      <c r="AB26" s="51"/>
-      <c r="AC26" s="51"/>
-      <c r="AD26" s="51"/>
-      <c r="AE26" s="51"/>
-      <c r="AF26" s="51"/>
-      <c r="AG26" s="51"/>
-      <c r="AH26" s="51"/>
-      <c r="AI26" s="51"/>
-      <c r="AJ26" s="51"/>
-      <c r="AK26" s="51"/>
-      <c r="AL26" s="51"/>
-      <c r="AM26" s="51"/>
-      <c r="AN26" s="51"/>
-      <c r="AO26" s="51"/>
-      <c r="AP26" s="51"/>
-      <c r="AQ26" s="51"/>
-      <c r="AR26" s="51"/>
-      <c r="AS26" s="51"/>
-      <c r="AT26" s="51"/>
-      <c r="AU26" s="51"/>
-      <c r="AV26" s="51"/>
-      <c r="AW26" s="51"/>
-      <c r="AX26" s="51"/>
-      <c r="AY26" s="51"/>
-      <c r="AZ26" s="51"/>
-      <c r="BA26" s="51"/>
-      <c r="BB26" s="51"/>
-      <c r="BC26" s="51"/>
-      <c r="BD26" s="51"/>
-      <c r="BE26" s="51"/>
-      <c r="BF26" s="51"/>
-      <c r="BG26" s="51"/>
-      <c r="BH26" s="51"/>
-      <c r="BI26" s="51"/>
-      <c r="BJ26" s="51"/>
-      <c r="BK26" s="51"/>
-      <c r="BL26" s="51"/>
+      <c r="I26" s="80"/>
+      <c r="J26" s="80"/>
+      <c r="K26" s="80"/>
+      <c r="L26" s="80"/>
+      <c r="M26" s="80"/>
+      <c r="N26" s="80"/>
+      <c r="O26" s="80"/>
+      <c r="P26" s="80"/>
+      <c r="Q26" s="80"/>
+      <c r="R26" s="80"/>
+      <c r="S26" s="80"/>
+      <c r="T26" s="80"/>
+      <c r="U26" s="80"/>
+      <c r="V26" s="80"/>
+      <c r="W26" s="80"/>
+      <c r="X26" s="80"/>
+      <c r="Y26" s="80"/>
+      <c r="Z26" s="80"/>
+      <c r="AA26" s="80"/>
+      <c r="AB26" s="80"/>
+      <c r="AC26" s="80"/>
+      <c r="AD26" s="80"/>
+      <c r="AE26" s="80"/>
+      <c r="AF26" s="80"/>
+      <c r="AG26" s="80"/>
+      <c r="AH26" s="80"/>
+      <c r="AI26" s="80"/>
+      <c r="AJ26" s="80"/>
+      <c r="AK26" s="80"/>
+      <c r="AL26" s="80"/>
+      <c r="AM26" s="80"/>
+      <c r="AN26" s="80"/>
+      <c r="AO26" s="80"/>
+      <c r="AP26" s="80"/>
+      <c r="AQ26" s="80"/>
+      <c r="AR26" s="80"/>
+      <c r="AS26" s="80"/>
+      <c r="AT26" s="80"/>
+      <c r="AU26" s="80"/>
+      <c r="AV26" s="80"/>
+      <c r="AW26" s="80"/>
+      <c r="AX26" s="80"/>
+      <c r="AY26" s="80"/>
+      <c r="AZ26" s="80"/>
+      <c r="BA26" s="80"/>
+      <c r="BB26" s="80"/>
+      <c r="BC26" s="80"/>
+      <c r="BD26" s="80"/>
+      <c r="BE26" s="80"/>
+      <c r="BF26" s="80"/>
+      <c r="BG26" s="80"/>
+      <c r="BH26" s="80"/>
+      <c r="BI26" s="80"/>
+      <c r="BJ26" s="80"/>
+      <c r="BK26" s="80"/>
+      <c r="BL26" s="80"/>
     </row>
     <row r="27" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="13"/>
       <c r="B27" s="81" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C27" s="82" t="s">
         <v>26</v>
@@ -3938,17 +3949,17 @@
         <v>0.05</v>
       </c>
       <c r="E27" s="84">
-        <f ca="1">F26</f>
-        <v>45265</v>
+        <f ca="1">E21+2</f>
+        <v>45266</v>
       </c>
       <c r="F27" s="84">
-        <f ca="1">E27+1</f>
-        <v>45266</v>
+        <f ca="1">E27+3</f>
+        <v>45269</v>
       </c>
       <c r="G27" s="17"/>
       <c r="H27" s="5">
         <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I27" s="51"/>
       <c r="J27" s="51"/>
@@ -4010,21 +4021,21 @@
     <row r="28" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="13"/>
       <c r="B28" s="81" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C28" s="82" t="s">
         <v>26</v>
       </c>
       <c r="D28" s="83">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E28" s="84">
-        <f ca="1">F27+1</f>
-        <v>45267</v>
+        <f ca="1">F27</f>
+        <v>45269</v>
       </c>
       <c r="F28" s="84">
         <f ca="1">E28+1</f>
-        <v>45268</v>
+        <v>45270</v>
       </c>
       <c r="G28" s="17"/>
       <c r="H28" s="5">
@@ -4091,21 +4102,21 @@
     <row r="29" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="13"/>
       <c r="B29" s="81" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C29" s="82" t="s">
         <v>26</v>
       </c>
       <c r="D29" s="83">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="E29" s="84">
-        <f ca="1">F28</f>
-        <v>45268</v>
+        <f ca="1">F28+1</f>
+        <v>45271</v>
       </c>
       <c r="F29" s="84">
         <f ca="1">E29+1</f>
-        <v>45269</v>
+        <v>45272</v>
       </c>
       <c r="G29" s="17"/>
       <c r="H29" s="5">
@@ -4172,26 +4183,26 @@
     <row r="30" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="13"/>
       <c r="B30" s="81" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C30" s="82" t="s">
         <v>26</v>
       </c>
       <c r="D30" s="83">
-        <v>0.1</v>
+        <v>0.33</v>
       </c>
       <c r="E30" s="84">
-        <f ca="1">E26</f>
-        <v>45262</v>
+        <f ca="1">F29</f>
+        <v>45272</v>
       </c>
       <c r="F30" s="84">
-        <f ca="1">F29</f>
-        <v>45269</v>
+        <f ca="1">E30+1</f>
+        <v>45273</v>
       </c>
       <c r="G30" s="17"/>
       <c r="H30" s="5">
         <f t="shared" ca="1" si="5"/>
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="I30" s="51"/>
       <c r="J30" s="51"/>
@@ -4252,153 +4263,234 @@
     </row>
     <row r="31" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="13"/>
-      <c r="B31" s="85"/>
-      <c r="C31" s="86"/>
-      <c r="D31" s="87"/>
-      <c r="E31" s="88"/>
-      <c r="F31" s="88"/>
+      <c r="B31" s="81" t="s">
+        <v>43</v>
+      </c>
+      <c r="C31" s="82" t="s">
+        <v>26</v>
+      </c>
+      <c r="D31" s="83">
+        <v>0.1</v>
+      </c>
+      <c r="E31" s="84">
+        <f ca="1">E27</f>
+        <v>45266</v>
+      </c>
+      <c r="F31" s="84">
+        <f ca="1">F30</f>
+        <v>45273</v>
+      </c>
       <c r="G31" s="17"/>
-      <c r="H31" s="5" t="str">
+      <c r="H31" s="5">
+        <f t="shared" ca="1" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="I31" s="51"/>
+      <c r="J31" s="51"/>
+      <c r="K31" s="51"/>
+      <c r="L31" s="51"/>
+      <c r="M31" s="51"/>
+      <c r="N31" s="51"/>
+      <c r="O31" s="51"/>
+      <c r="P31" s="51"/>
+      <c r="Q31" s="51"/>
+      <c r="R31" s="51"/>
+      <c r="S31" s="51"/>
+      <c r="T31" s="51"/>
+      <c r="U31" s="51"/>
+      <c r="V31" s="51"/>
+      <c r="W31" s="51"/>
+      <c r="X31" s="51"/>
+      <c r="Y31" s="51"/>
+      <c r="Z31" s="51"/>
+      <c r="AA31" s="51"/>
+      <c r="AB31" s="51"/>
+      <c r="AC31" s="51"/>
+      <c r="AD31" s="51"/>
+      <c r="AE31" s="51"/>
+      <c r="AF31" s="51"/>
+      <c r="AG31" s="51"/>
+      <c r="AH31" s="51"/>
+      <c r="AI31" s="51"/>
+      <c r="AJ31" s="51"/>
+      <c r="AK31" s="51"/>
+      <c r="AL31" s="51"/>
+      <c r="AM31" s="51"/>
+      <c r="AN31" s="51"/>
+      <c r="AO31" s="51"/>
+      <c r="AP31" s="51"/>
+      <c r="AQ31" s="51"/>
+      <c r="AR31" s="51"/>
+      <c r="AS31" s="51"/>
+      <c r="AT31" s="51"/>
+      <c r="AU31" s="51"/>
+      <c r="AV31" s="51"/>
+      <c r="AW31" s="51"/>
+      <c r="AX31" s="51"/>
+      <c r="AY31" s="51"/>
+      <c r="AZ31" s="51"/>
+      <c r="BA31" s="51"/>
+      <c r="BB31" s="51"/>
+      <c r="BC31" s="51"/>
+      <c r="BD31" s="51"/>
+      <c r="BE31" s="51"/>
+      <c r="BF31" s="51"/>
+      <c r="BG31" s="51"/>
+      <c r="BH31" s="51"/>
+      <c r="BI31" s="51"/>
+      <c r="BJ31" s="51"/>
+      <c r="BK31" s="51"/>
+      <c r="BL31" s="51"/>
+    </row>
+    <row r="32" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="13"/>
+      <c r="B32" s="85"/>
+      <c r="C32" s="86"/>
+      <c r="D32" s="87"/>
+      <c r="E32" s="88"/>
+      <c r="F32" s="88"/>
+      <c r="G32" s="17"/>
+      <c r="H32" s="5" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="I31" s="45"/>
-      <c r="J31" s="45"/>
-      <c r="K31" s="45"/>
-      <c r="L31" s="45"/>
-      <c r="M31" s="45"/>
-      <c r="N31" s="45"/>
-      <c r="O31" s="45"/>
-      <c r="P31" s="45"/>
-      <c r="Q31" s="45"/>
-      <c r="R31" s="45"/>
-      <c r="S31" s="45"/>
-      <c r="T31" s="45"/>
-      <c r="U31" s="45"/>
-      <c r="V31" s="45"/>
-      <c r="W31" s="45"/>
-      <c r="X31" s="45"/>
-      <c r="Y31" s="45"/>
-      <c r="Z31" s="45"/>
-      <c r="AA31" s="45"/>
-      <c r="AB31" s="45"/>
-      <c r="AC31" s="45"/>
-      <c r="AD31" s="45"/>
-      <c r="AE31" s="45"/>
-      <c r="AF31" s="45"/>
-      <c r="AG31" s="45"/>
-      <c r="AH31" s="45"/>
-      <c r="AI31" s="45"/>
-      <c r="AJ31" s="45"/>
-      <c r="AK31" s="45"/>
-      <c r="AL31" s="45"/>
-      <c r="AM31" s="45"/>
-      <c r="AN31" s="45"/>
-      <c r="AO31" s="45"/>
-      <c r="AP31" s="45"/>
-      <c r="AQ31" s="45"/>
-      <c r="AR31" s="45"/>
-      <c r="AS31" s="45"/>
-      <c r="AT31" s="45"/>
-      <c r="AU31" s="45"/>
-      <c r="AV31" s="45"/>
-      <c r="AW31" s="45"/>
-      <c r="AX31" s="45"/>
-      <c r="AY31" s="45"/>
-      <c r="AZ31" s="45"/>
-      <c r="BA31" s="45"/>
-      <c r="BB31" s="45"/>
-      <c r="BC31" s="45"/>
-      <c r="BD31" s="45"/>
-      <c r="BE31" s="45"/>
-      <c r="BF31" s="45"/>
-      <c r="BG31" s="45"/>
-      <c r="BH31" s="45"/>
-      <c r="BI31" s="45"/>
-      <c r="BJ31" s="45"/>
-      <c r="BK31" s="45"/>
-      <c r="BL31" s="45"/>
-    </row>
-    <row r="32" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="14"/>
-      <c r="B32" s="89" t="s">
+      <c r="I32" s="45"/>
+      <c r="J32" s="45"/>
+      <c r="K32" s="45"/>
+      <c r="L32" s="45"/>
+      <c r="M32" s="45"/>
+      <c r="N32" s="45"/>
+      <c r="O32" s="45"/>
+      <c r="P32" s="45"/>
+      <c r="Q32" s="45"/>
+      <c r="R32" s="45"/>
+      <c r="S32" s="45"/>
+      <c r="T32" s="45"/>
+      <c r="U32" s="45"/>
+      <c r="V32" s="45"/>
+      <c r="W32" s="45"/>
+      <c r="X32" s="45"/>
+      <c r="Y32" s="45"/>
+      <c r="Z32" s="45"/>
+      <c r="AA32" s="45"/>
+      <c r="AB32" s="45"/>
+      <c r="AC32" s="45"/>
+      <c r="AD32" s="45"/>
+      <c r="AE32" s="45"/>
+      <c r="AF32" s="45"/>
+      <c r="AG32" s="45"/>
+      <c r="AH32" s="45"/>
+      <c r="AI32" s="45"/>
+      <c r="AJ32" s="45"/>
+      <c r="AK32" s="45"/>
+      <c r="AL32" s="45"/>
+      <c r="AM32" s="45"/>
+      <c r="AN32" s="45"/>
+      <c r="AO32" s="45"/>
+      <c r="AP32" s="45"/>
+      <c r="AQ32" s="45"/>
+      <c r="AR32" s="45"/>
+      <c r="AS32" s="45"/>
+      <c r="AT32" s="45"/>
+      <c r="AU32" s="45"/>
+      <c r="AV32" s="45"/>
+      <c r="AW32" s="45"/>
+      <c r="AX32" s="45"/>
+      <c r="AY32" s="45"/>
+      <c r="AZ32" s="45"/>
+      <c r="BA32" s="45"/>
+      <c r="BB32" s="45"/>
+      <c r="BC32" s="45"/>
+      <c r="BD32" s="45"/>
+      <c r="BE32" s="45"/>
+      <c r="BF32" s="45"/>
+      <c r="BG32" s="45"/>
+      <c r="BH32" s="45"/>
+      <c r="BI32" s="45"/>
+      <c r="BJ32" s="45"/>
+      <c r="BK32" s="45"/>
+      <c r="BL32" s="45"/>
+    </row>
+    <row r="33" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="14"/>
+      <c r="B33" s="89" t="s">
         <v>0</v>
       </c>
-      <c r="C32" s="90"/>
-      <c r="D32" s="91"/>
-      <c r="E32" s="92"/>
-      <c r="F32" s="93"/>
-      <c r="G32" s="17"/>
-      <c r="H32" s="6" t="str">
+      <c r="C33" s="90"/>
+      <c r="D33" s="91"/>
+      <c r="E33" s="92"/>
+      <c r="F33" s="93"/>
+      <c r="G33" s="17"/>
+      <c r="H33" s="6" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="I32" s="94"/>
-      <c r="J32" s="94"/>
-      <c r="K32" s="94"/>
-      <c r="L32" s="94"/>
-      <c r="M32" s="94"/>
-      <c r="N32" s="94"/>
-      <c r="O32" s="94"/>
-      <c r="P32" s="94"/>
-      <c r="Q32" s="94"/>
-      <c r="R32" s="94"/>
-      <c r="S32" s="94"/>
-      <c r="T32" s="94"/>
-      <c r="U32" s="94"/>
-      <c r="V32" s="94"/>
-      <c r="W32" s="94"/>
-      <c r="X32" s="94"/>
-      <c r="Y32" s="94"/>
-      <c r="Z32" s="94"/>
-      <c r="AA32" s="94"/>
-      <c r="AB32" s="94"/>
-      <c r="AC32" s="94"/>
-      <c r="AD32" s="94"/>
-      <c r="AE32" s="94"/>
-      <c r="AF32" s="94"/>
-      <c r="AG32" s="94"/>
-      <c r="AH32" s="94"/>
-      <c r="AI32" s="94"/>
-      <c r="AJ32" s="94"/>
-      <c r="AK32" s="94"/>
-      <c r="AL32" s="94"/>
-      <c r="AM32" s="94"/>
-      <c r="AN32" s="94"/>
-      <c r="AO32" s="94"/>
-      <c r="AP32" s="94"/>
-      <c r="AQ32" s="94"/>
-      <c r="AR32" s="94"/>
-      <c r="AS32" s="94"/>
-      <c r="AT32" s="94"/>
-      <c r="AU32" s="94"/>
-      <c r="AV32" s="94"/>
-      <c r="AW32" s="94"/>
-      <c r="AX32" s="94"/>
-      <c r="AY32" s="94"/>
-      <c r="AZ32" s="94"/>
-      <c r="BA32" s="94"/>
-      <c r="BB32" s="94"/>
-      <c r="BC32" s="94"/>
-      <c r="BD32" s="94"/>
-      <c r="BE32" s="94"/>
-      <c r="BF32" s="94"/>
-      <c r="BG32" s="94"/>
-      <c r="BH32" s="94"/>
-      <c r="BI32" s="94"/>
-      <c r="BJ32" s="94"/>
-      <c r="BK32" s="94"/>
-      <c r="BL32" s="94"/>
-    </row>
-    <row r="33" spans="3:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G33" s="3"/>
-    </row>
-    <row r="34" spans="3:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C34" s="16"/>
-      <c r="F34" s="15"/>
-    </row>
-    <row r="35" spans="3:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C35" s="4"/>
+      <c r="I33" s="94"/>
+      <c r="J33" s="94"/>
+      <c r="K33" s="94"/>
+      <c r="L33" s="94"/>
+      <c r="M33" s="94"/>
+      <c r="N33" s="94"/>
+      <c r="O33" s="94"/>
+      <c r="P33" s="94"/>
+      <c r="Q33" s="94"/>
+      <c r="R33" s="94"/>
+      <c r="S33" s="94"/>
+      <c r="T33" s="94"/>
+      <c r="U33" s="94"/>
+      <c r="V33" s="94"/>
+      <c r="W33" s="94"/>
+      <c r="X33" s="94"/>
+      <c r="Y33" s="94"/>
+      <c r="Z33" s="94"/>
+      <c r="AA33" s="94"/>
+      <c r="AB33" s="94"/>
+      <c r="AC33" s="94"/>
+      <c r="AD33" s="94"/>
+      <c r="AE33" s="94"/>
+      <c r="AF33" s="94"/>
+      <c r="AG33" s="94"/>
+      <c r="AH33" s="94"/>
+      <c r="AI33" s="94"/>
+      <c r="AJ33" s="94"/>
+      <c r="AK33" s="94"/>
+      <c r="AL33" s="94"/>
+      <c r="AM33" s="94"/>
+      <c r="AN33" s="94"/>
+      <c r="AO33" s="94"/>
+      <c r="AP33" s="94"/>
+      <c r="AQ33" s="94"/>
+      <c r="AR33" s="94"/>
+      <c r="AS33" s="94"/>
+      <c r="AT33" s="94"/>
+      <c r="AU33" s="94"/>
+      <c r="AV33" s="94"/>
+      <c r="AW33" s="94"/>
+      <c r="AX33" s="94"/>
+      <c r="AY33" s="94"/>
+      <c r="AZ33" s="94"/>
+      <c r="BA33" s="94"/>
+      <c r="BB33" s="94"/>
+      <c r="BC33" s="94"/>
+      <c r="BD33" s="94"/>
+      <c r="BE33" s="94"/>
+      <c r="BF33" s="94"/>
+      <c r="BG33" s="94"/>
+      <c r="BH33" s="94"/>
+      <c r="BI33" s="94"/>
+      <c r="BJ33" s="94"/>
+      <c r="BK33" s="94"/>
+      <c r="BL33" s="94"/>
+    </row>
+    <row r="34" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G34" s="3"/>
+    </row>
+    <row r="35" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C35" s="16"/>
+      <c r="F35" s="15"/>
+    </row>
+    <row r="36" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C36" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="18">
@@ -4421,7 +4513,7 @@
     <mergeCell ref="D5:D6"/>
     <mergeCell ref="E5:E6"/>
   </mergeCells>
-  <conditionalFormatting sqref="D7:D32">
+  <conditionalFormatting sqref="D7:D33">
     <cfRule type="dataBar" priority="23">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -4443,7 +4535,7 @@
       <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I13:BL17">
+  <conditionalFormatting sqref="I13:BL18">
     <cfRule type="expression" dxfId="6" priority="4">
       <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
     </cfRule>
@@ -4451,7 +4543,7 @@
       <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I19:BL24">
+  <conditionalFormatting sqref="I20:BL25">
     <cfRule type="expression" dxfId="4" priority="2">
       <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
     </cfRule>
@@ -4459,7 +4551,7 @@
       <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I26:BL30">
+  <conditionalFormatting sqref="I27:BL31">
     <cfRule type="expression" dxfId="2" priority="36">
       <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
     </cfRule>
@@ -4467,7 +4559,7 @@
       <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I4:BL30">
+  <conditionalFormatting sqref="I4:BL31">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>AND(TODAY()&gt;=I$5, TODAY()&lt;J$5)</formula>
     </cfRule>
@@ -4485,9 +4577,9 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="B9 contains the task name.  C9 is the assignee.  D9 is a progress bar that shades based on the number entered into the cell.  _x000a__x000a_E9 contains the start date and F9 contains the end date._x000a__x000a_The Gantt chart will fill in starting in cell I9 based on task dates." sqref="A9" xr:uid="{D870A2F6-6B07-4F5A-A81D-4BCCFADF8796}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Rows 10 through 13 repeat the pattern from row 9. _x000a__x000a_Repeat the instructions from cell A9 for all task rows in this worksheet. _x000a__x000a_Continue entering tasks in cells A10 through A13 or go to cell A14 to learn more." sqref="A10" xr:uid="{872449A7-C3CC-45B6-BA90-B1AAD66BA0E5}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Cell B14 contains the Phase 2 sample title. Enter a new title in cell B14._x000a_To delete the phase and work only from tasks, simply delete this row. To remove the phase, simply delete the row. Add tasks to previous phase by entering a new row above this one._x000a_" sqref="A12" xr:uid="{4F48FC41-E335-47F1-87AA-3333A52AD81C}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Phase 3's sample block starts in cell B20." sqref="A18" xr:uid="{956902D1-D3B5-416D-BB69-9362D193BC0A}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Phase 4's sample block starts in cell B26." sqref="A25" xr:uid="{DE54E5DE-526D-4D71-8D03-E99B4AB2FEE5}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This row marks the end of the Project Schedule. DO NOT enter anything in this row. _x000a_Insert new rows ABOVE this one to continue building out your Project Schedule." sqref="A32" xr:uid="{79B9237E-4DD3-4E0F-8ED6-E0B695A99D96}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Phase 3's sample block starts in cell B20." sqref="A19" xr:uid="{956902D1-D3B5-416D-BB69-9362D193BC0A}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Phase 4's sample block starts in cell B26." sqref="A26" xr:uid="{DE54E5DE-526D-4D71-8D03-E99B4AB2FEE5}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This row marks the end of the Project Schedule. DO NOT enter anything in this row. _x000a_Insert new rows ABOVE this one to continue building out your Project Schedule." sqref="A33" xr:uid="{79B9237E-4DD3-4E0F-8ED6-E0B695A99D96}"/>
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="B4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -4516,7 +4608,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D7:D32</xm:sqref>
+          <xm:sqref>D7:D33</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>